<commit_message>
improvements to EXCELL sheet
</commit_message>
<xml_diff>
--- a/Score.xlsx
+++ b/Score.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Day</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVERAGE</t>
   </si>
   <si>
     <t xml:space="preserve">Stars</t>
@@ -45,11 +48,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -66,6 +70,11 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -77,7 +86,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FFB3B3B3"/>
       </patternFill>
     </fill>
     <fill>
@@ -159,7 +168,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -188,12 +197,12 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -206,18 +215,611 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$Z$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lines/code</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$Z$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time(min)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$Z$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="93462329"/>
+        <c:axId val="1562930"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="93462329"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1562930"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1562930"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93462329"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15120</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="820080"/>
+        <a:ext cx="5760720" cy="3236400"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="6.35"/>
   </cols>
@@ -304,10 +906,13 @@
       <c r="AA1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -386,12 +991,16 @@
       </c>
       <c r="AA2" s="2" t="n">
         <f aca="false">SUM(B2:Z2)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <f aca="false">AVERAGE(B2:Z2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -470,12 +1079,16 @@
       </c>
       <c r="AA3" s="2" t="n">
         <f aca="false">SUM(B3:Z3)</f>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <f aca="false">AVERAGE(B3:Z3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -554,6 +1167,10 @@
       </c>
       <c r="AA4" s="2" t="n">
         <f aca="false">SUM(B4:Z4)</f>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <f aca="false">AVERAGE(B4:Z4)</f>
         <v>0</v>
       </c>
     </row>
@@ -565,5 +1182,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor tweaks to score.xlsx
</commit_message>
<xml_diff>
--- a/Score.xlsx
+++ b/Score.xlsx
@@ -218,7 +218,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -656,11 +656,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="40398275"/>
-        <c:axId val="39445448"/>
+        <c:axId val="47592150"/>
+        <c:axId val="95432496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40398275"/>
+        <c:axId val="47592150"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +688,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39445448"/>
+        <c:crossAx val="95432496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39445448"/>
+        <c:axId val="95432496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,7 +733,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40398275"/>
+        <c:crossAx val="47592150"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -790,9 +790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>14760</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -801,7 +801,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="820080"/>
-        <a:ext cx="5761440" cy="3236040"/>
+        <a:ext cx="5762520" cy="3235680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -822,10 +822,10 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="6.35"/>
   </cols>
@@ -1009,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
-        <f aca="false">SUM(37, 71)</f>
+        <f aca="false">37+71</f>
         <v>108</v>
       </c>
       <c r="C3" s="0" t="n">

</xml_diff>

<commit_message>
day2 p1 is done!
</commit_message>
<xml_diff>
--- a/Score.xlsx
+++ b/Score.xlsx
@@ -133,16 +133,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,7 +296,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -432,7 +436,7 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -572,7 +576,7 @@
                   <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -656,11 +660,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="47592150"/>
-        <c:axId val="95432496"/>
+        <c:axId val="16733095"/>
+        <c:axId val="61259055"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47592150"/>
+        <c:axId val="16733095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +692,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95432496"/>
+        <c:crossAx val="61259055"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95432496"/>
+        <c:axId val="61259055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,7 +737,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47592150"/>
+        <c:crossAx val="16733095"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -790,9 +794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>14040</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -801,7 +805,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="820080"/>
-        <a:ext cx="5762520" cy="3235680"/>
+        <a:ext cx="5754960" cy="3235320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -815,375 +819,375 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="6.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="1" width="6.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="2" t="n">
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3" t="n">
         <f aca="false">SUM(B2:Z2)</f>
-        <v>2</v>
-      </c>
-      <c r="AB2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="3" t="n">
         <f aca="false">AVERAGE(B2:Z2)</f>
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">37+71</f>
         <v>108</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2" t="n">
+      <c r="C3" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3" t="n">
         <f aca="false">SUM(B3:Z3)</f>
-        <v>108</v>
-      </c>
-      <c r="AB3" s="2" t="n">
+        <v>198</v>
+      </c>
+      <c r="AB3" s="3" t="n">
         <f aca="false">AVERAGE(B3:Z3)</f>
-        <v>4.32</v>
+        <v>7.92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">4*60</f>
         <v>240</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="2" t="n">
+      <c r="C4" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3" t="n">
         <f aca="false">SUM(B4:Z4)</f>
-        <v>240</v>
-      </c>
-      <c r="AB4" s="2" t="n">
+        <v>285</v>
+      </c>
+      <c r="AB4" s="3" t="n">
         <f aca="false">AVERAGE(B4:Z4)</f>
-        <v>9.6</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>